<commit_message>
adding output and requirements
</commit_message>
<xml_diff>
--- a/outputs/protocol_summary.xlsx
+++ b/outputs/protocol_summary.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V3"/>
+  <dimension ref="A1:V13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -604,32 +604,32 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2025-10-27</t>
+          <t>2025-10-19</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>70.9</t>
+          <t>71.2</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>24.5</t>
+          <t>25.2</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>51.8</t>
+          <t>51.5</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>39.5</t>
+          <t>39.3</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>2.8</t>
+          <t>2.7</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
@@ -654,48 +654,1052 @@
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>2258</t>
+          <t>1959</t>
         </is>
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>157</t>
+          <t>141</t>
         </is>
       </c>
       <c r="M3" t="inlineStr">
         <is>
-          <t>84</t>
+          <t>51</t>
         </is>
       </c>
       <c r="N3" t="inlineStr">
         <is>
-          <t>184</t>
+          <t>214</t>
         </is>
       </c>
       <c r="O3" t="inlineStr">
         <is>
-          <t>101</t>
+          <t>None</t>
         </is>
       </c>
       <c r="P3" t="inlineStr">
         <is>
-          <t>7.40</t>
-        </is>
-      </c>
-      <c r="Q3" t="inlineStr"/>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="Q3" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
       <c r="R3" t="inlineStr">
         <is>
-          <t>Home</t>
+          <t>None</t>
         </is>
       </c>
       <c r="S3" t="inlineStr">
         <is>
-          <t>25.1</t>
+          <t>25.2</t>
         </is>
       </c>
       <c r="T3" t="inlineStr"/>
       <c r="U3" t="inlineStr"/>
       <c r="V3" t="inlineStr"/>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>2025-10-20</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>71.2</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>25.8</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>51.1</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>39.1</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>2.7</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>2300</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>150</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>80</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>240</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>1966</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>143</t>
+        </is>
+      </c>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>101</t>
+        </is>
+      </c>
+      <c r="N4" t="inlineStr">
+        <is>
+          <t>107</t>
+        </is>
+      </c>
+      <c r="O4" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="P4" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="Q4" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="R4" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="S4" t="inlineStr">
+        <is>
+          <t>25.2</t>
+        </is>
+      </c>
+      <c r="T4" t="inlineStr"/>
+      <c r="U4" t="inlineStr"/>
+      <c r="V4" t="inlineStr"/>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>2025-10-21</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>70.2</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>24.3</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>52</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>39.6</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>2.7</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>2300</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>150</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>80</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>240</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>1981</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>129</t>
+        </is>
+      </c>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>88</t>
+        </is>
+      </c>
+      <c r="N5" t="inlineStr">
+        <is>
+          <t>153</t>
+        </is>
+      </c>
+      <c r="O5" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="P5" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="Q5" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="R5" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="S5" t="inlineStr">
+        <is>
+          <t>24.8</t>
+        </is>
+      </c>
+      <c r="T5" t="inlineStr"/>
+      <c r="U5" t="inlineStr"/>
+      <c r="V5" t="inlineStr"/>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>2025-10-22</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>70.3</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>24</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>52.2</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>39.7</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>2.8</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>2300</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>150</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>80</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>240</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>2030</t>
+        </is>
+      </c>
+      <c r="L6" t="inlineStr">
+        <is>
+          <t>144</t>
+        </is>
+      </c>
+      <c r="M6" t="inlineStr">
+        <is>
+          <t>84</t>
+        </is>
+      </c>
+      <c r="N6" t="inlineStr">
+        <is>
+          <t>154</t>
+        </is>
+      </c>
+      <c r="O6" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="P6" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="Q6" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="R6" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="S6" t="inlineStr">
+        <is>
+          <t>24.8</t>
+        </is>
+      </c>
+      <c r="T6" t="inlineStr"/>
+      <c r="U6" t="inlineStr"/>
+      <c r="V6" t="inlineStr"/>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>2025-10-23</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>70.6</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>24.8</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>51.7</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>39.5</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>2.7</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>2300</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>150</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>80</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>240</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>2736</t>
+        </is>
+      </c>
+      <c r="L7" t="inlineStr">
+        <is>
+          <t>159</t>
+        </is>
+      </c>
+      <c r="M7" t="inlineStr">
+        <is>
+          <t>131</t>
+        </is>
+      </c>
+      <c r="N7" t="inlineStr">
+        <is>
+          <t>214</t>
+        </is>
+      </c>
+      <c r="O7" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="P7" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="Q7" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="R7" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="S7" t="inlineStr">
+        <is>
+          <t>25</t>
+        </is>
+      </c>
+      <c r="T7" t="inlineStr"/>
+      <c r="U7" t="inlineStr"/>
+      <c r="V7" t="inlineStr"/>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>2025-10-24</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>70.9</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>25.6</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>51.3</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>39.2</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>2.7</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>2300</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>150</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>80</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>240</t>
+        </is>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>2173</t>
+        </is>
+      </c>
+      <c r="L8" t="inlineStr">
+        <is>
+          <t>184</t>
+        </is>
+      </c>
+      <c r="M8" t="inlineStr">
+        <is>
+          <t>84</t>
+        </is>
+      </c>
+      <c r="N8" t="inlineStr">
+        <is>
+          <t>156</t>
+        </is>
+      </c>
+      <c r="O8" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="P8" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="Q8" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="R8" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="S8" t="inlineStr">
+        <is>
+          <t>25.1</t>
+        </is>
+      </c>
+      <c r="T8" t="inlineStr"/>
+      <c r="U8" t="inlineStr"/>
+      <c r="V8" t="inlineStr"/>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>2025-10-25</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>71.6</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>25.5</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>51.2</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>39.2</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>2.8</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>2300</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>150</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>80</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>240</t>
+        </is>
+      </c>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>2177</t>
+        </is>
+      </c>
+      <c r="L9" t="inlineStr">
+        <is>
+          <t>97</t>
+        </is>
+      </c>
+      <c r="M9" t="inlineStr">
+        <is>
+          <t>106</t>
+        </is>
+      </c>
+      <c r="N9" t="inlineStr">
+        <is>
+          <t>224</t>
+        </is>
+      </c>
+      <c r="O9" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="P9" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="Q9" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="R9" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="S9" t="inlineStr">
+        <is>
+          <t>25.3</t>
+        </is>
+      </c>
+      <c r="T9" t="inlineStr"/>
+      <c r="U9" t="inlineStr"/>
+      <c r="V9" t="inlineStr"/>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>2025-10-26</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>2300</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>150</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>80</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>240</t>
+        </is>
+      </c>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>2139</t>
+        </is>
+      </c>
+      <c r="L10" t="inlineStr">
+        <is>
+          <t>108</t>
+        </is>
+      </c>
+      <c r="M10" t="inlineStr">
+        <is>
+          <t>107</t>
+        </is>
+      </c>
+      <c r="N10" t="inlineStr">
+        <is>
+          <t>187</t>
+        </is>
+      </c>
+      <c r="O10" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="P10" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="Q10" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="R10" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="S10" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="T10" t="inlineStr"/>
+      <c r="U10" t="inlineStr"/>
+      <c r="V10" t="inlineStr"/>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>2025-10-27</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>70.9</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>24.5</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>51.8</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>39.5</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>2.8</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>2300</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>150</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>80</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>240</t>
+        </is>
+      </c>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>2258</t>
+        </is>
+      </c>
+      <c r="L11" t="inlineStr">
+        <is>
+          <t>157</t>
+        </is>
+      </c>
+      <c r="M11" t="inlineStr">
+        <is>
+          <t>84</t>
+        </is>
+      </c>
+      <c r="N11" t="inlineStr">
+        <is>
+          <t>184</t>
+        </is>
+      </c>
+      <c r="O11" t="inlineStr">
+        <is>
+          <t>101</t>
+        </is>
+      </c>
+      <c r="P11" t="inlineStr">
+        <is>
+          <t>7h 24m</t>
+        </is>
+      </c>
+      <c r="Q11" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="R11" t="inlineStr">
+        <is>
+          <t>Home</t>
+        </is>
+      </c>
+      <c r="S11" t="inlineStr">
+        <is>
+          <t>25.1</t>
+        </is>
+      </c>
+      <c r="T11" t="inlineStr"/>
+      <c r="U11" t="inlineStr"/>
+      <c r="V11" t="inlineStr"/>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>2025-10-28</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>71.2</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>25.5</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>51.3</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>39.2</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>2.7</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>2300</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>150</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>80</t>
+        </is>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>240</t>
+        </is>
+      </c>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>2255</t>
+        </is>
+      </c>
+      <c r="L12" t="inlineStr">
+        <is>
+          <t>157</t>
+        </is>
+      </c>
+      <c r="M12" t="inlineStr">
+        <is>
+          <t>84</t>
+        </is>
+      </c>
+      <c r="N12" t="inlineStr">
+        <is>
+          <t>184</t>
+        </is>
+      </c>
+      <c r="O12" t="inlineStr">
+        <is>
+          <t>102</t>
+        </is>
+      </c>
+      <c r="P12" t="inlineStr">
+        <is>
+          <t>438</t>
+        </is>
+      </c>
+      <c r="Q12" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="R12" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="S12" t="inlineStr">
+        <is>
+          <t>25.2</t>
+        </is>
+      </c>
+      <c r="T12" t="inlineStr"/>
+      <c r="U12" t="inlineStr"/>
+      <c r="V12" t="inlineStr"/>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>2025-10-29</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>72.1</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>25</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>51.4</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>39.3</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>2.8</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>2300</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>150</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>80</t>
+        </is>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>240</t>
+        </is>
+      </c>
+      <c r="K13" t="inlineStr">
+        <is>
+          <t>2432</t>
+        </is>
+      </c>
+      <c r="L13" t="inlineStr">
+        <is>
+          <t>183</t>
+        </is>
+      </c>
+      <c r="M13" t="inlineStr">
+        <is>
+          <t>81</t>
+        </is>
+      </c>
+      <c r="N13" t="inlineStr">
+        <is>
+          <t>223</t>
+        </is>
+      </c>
+      <c r="O13" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="P13" t="inlineStr">
+        <is>
+          <t>326</t>
+        </is>
+      </c>
+      <c r="Q13" t="inlineStr">
+        <is>
+          <t>6342</t>
+        </is>
+      </c>
+      <c r="R13" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="S13" t="inlineStr">
+        <is>
+          <t>25.5</t>
+        </is>
+      </c>
+      <c r="T13" t="inlineStr"/>
+      <c r="U13" t="inlineStr"/>
+      <c r="V13" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>